<commit_message>
From bjo-sea01 init client 2023-11-28.153208
</commit_message>
<xml_diff>
--- a/config/config/role-structure.SEA01.xlsx
+++ b/config/config/role-structure.SEA01.xlsx
@@ -1,19 +1,19 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10917"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11116"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/personal/Documents/docker/data/client/ysh/client/lnw-xdt01/config/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/personal/Documents/docker/data/client/ysh/client/bjo-sea01/config/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5229B910-F589-B24C-9D29-143D8EA23768}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{82B50294-8A56-294C-A621-55CAB8D5211E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7420" yWindow="11640" windowWidth="16160" windowHeight="11400" xr2:uid="{D1E400A9-94D3-C340-ADBB-65EA67C8B266}"/>
+    <workbookView xWindow="19000" yWindow="5660" windowWidth="16160" windowHeight="11400" xr2:uid="{D1E400A9-94D3-C340-ADBB-65EA67C8B266}"/>
   </bookViews>
   <sheets>
-    <sheet name="NONE" sheetId="3" r:id="rId1"/>
+    <sheet name="USER_LIST" sheetId="4" r:id="rId1"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -22,6 +22,29 @@
     </ext>
   </extLst>
 </workbook>
+</file>
+
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="6">
+  <si>
+    <t>*END*</t>
+  </si>
+  <si>
+    <t>User</t>
+  </si>
+  <si>
+    <t>User Group</t>
+  </si>
+  <si>
+    <t>LEO</t>
+  </si>
+  <si>
+    <t>CLIENT_ADMIN</t>
+  </si>
+  <si>
+    <t>NEMOO</t>
+  </si>
+</sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
@@ -370,13 +393,49 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{04034489-2E83-734A-8940-45A53E3AC516}">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A95348D2-1418-AA40-B4AA-D28C48AAAB7F}">
+  <dimension ref="A1:B4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A5" sqref="A4:XFD5"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="11.83203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.6640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
From bjo-sea01 add seamless01 2023-11-28.184652
</commit_message>
<xml_diff>
--- a/config/config/role-structure.SEA01.xlsx
+++ b/config/config/role-structure.SEA01.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/personal/Documents/docker/data/client/ysh/client/bjo-sea01/config/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{82B50294-8A56-294C-A621-55CAB8D5211E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{27094B15-EDD2-DA48-806A-4364F73F781E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="19000" yWindow="5660" windowWidth="16160" windowHeight="11400" xr2:uid="{D1E400A9-94D3-C340-ADBB-65EA67C8B266}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="7">
   <si>
     <t>*END*</t>
   </si>
@@ -43,6 +43,9 @@
   </si>
   <si>
     <t>NEMOO</t>
+  </si>
+  <si>
+    <t>SEAMLESS01</t>
   </si>
 </sst>
 </file>
@@ -394,16 +397,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A95348D2-1418-AA40-B4AA-D28C48AAAB7F}">
-  <dimension ref="A1:B4"/>
+  <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A5" sqref="A4:XFD5"/>
+      <selection activeCell="B9" activeCellId="1" sqref="B4 B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="11.83203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="15.6640625" customWidth="1"/>
+    <col min="2" max="2" width="18" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
@@ -432,6 +435,14 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
         <v>0</v>
       </c>
     </row>

</xml_diff>